<commit_message>
refactor/DinerExcelServiceImpl - Add refineCategory method in DinerExcelServiceImpl.java - Add DinerListController and DTO for Dinner - Add link to Diner List page in index.html - Add method to fetch diner list in DinerService and DinerServiceImpl.java - Modify DinerRepository to support fetching diner list - Create dinerList.html for displaying diner list
</commit_message>
<xml_diff>
--- a/src/main/resources/test_diner.xlsx
+++ b/src/main/resources/test_diner.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KH302\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dcf6b2c3f1f2c6e2/Desktop/table_grap_lyj/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2121E8B2-6482-4EB8-B86E-4BA33DCAB468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{2121E8B2-6482-4EB8-B86E-4BA33DCAB468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6A71DBE-E94E-461C-9905-E0F33985C64C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{185B2E48-665A-43A7-A2B2-8C1EA9FB939C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{185B2E48-665A-43A7-A2B2-8C1EA9FB939C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="513">
   <si>
     <t>번호</t>
   </si>
@@ -586,6 +588,993 @@
   </si>
   <si>
     <t>2023-12-30 02:40:00</t>
+  </si>
+  <si>
+    <t>11209</t>
+  </si>
+  <si>
+    <t>3700000</t>
+  </si>
+  <si>
+    <t>3700000-101-2009-00193</t>
+  </si>
+  <si>
+    <t>2009-06-16</t>
+  </si>
+  <si>
+    <t>052 269 5412</t>
+  </si>
+  <si>
+    <t>6.50</t>
+  </si>
+  <si>
+    <t>680-839</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 남구 야음동 698-14 </t>
+  </si>
+  <si>
+    <t>울산광역시 남구 수암로 120-3, 1층 (야음동)</t>
+  </si>
+  <si>
+    <t>44749</t>
+  </si>
+  <si>
+    <t>벌통식당</t>
+  </si>
+  <si>
+    <t>2023-05-03 17:43:39</t>
+  </si>
+  <si>
+    <t>2023-05-05 02:40:00</t>
+  </si>
+  <si>
+    <t>11414</t>
+  </si>
+  <si>
+    <t>3700000-101-2012-00208</t>
+  </si>
+  <si>
+    <t>2012-08-17</t>
+  </si>
+  <si>
+    <t>052  2737374</t>
+  </si>
+  <si>
+    <t>43.65</t>
+  </si>
+  <si>
+    <t>680-834</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 남구 야음동 282-5번지 </t>
+  </si>
+  <si>
+    <t>울산광역시 남구 여천로12번길 21, 1층 (야음동)</t>
+  </si>
+  <si>
+    <t>44766</t>
+  </si>
+  <si>
+    <t>마산식당</t>
+  </si>
+  <si>
+    <t>2017-08-09 15:42:32</t>
+  </si>
+  <si>
+    <t>11431</t>
+  </si>
+  <si>
+    <t>3700000-101-2005-00402</t>
+  </si>
+  <si>
+    <t>2005-11-17</t>
+  </si>
+  <si>
+    <t>2669291</t>
+  </si>
+  <si>
+    <t>129.05</t>
+  </si>
+  <si>
+    <t>680-815</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 남구 삼산동 1643-7 (지상1층) </t>
+  </si>
+  <si>
+    <t>울산광역시 남구 산업로647번길 9 (삼산동,(지상1층))</t>
+  </si>
+  <si>
+    <t>44716</t>
+  </si>
+  <si>
+    <t>따꿍식당</t>
+  </si>
+  <si>
+    <t>2025-09-24 14:26:12</t>
+  </si>
+  <si>
+    <t>2025-09-26 02:40:00</t>
+  </si>
+  <si>
+    <t>11501</t>
+  </si>
+  <si>
+    <t>3700000-101-2006-00178</t>
+  </si>
+  <si>
+    <t>2006-05-16</t>
+  </si>
+  <si>
+    <t>052 2763057</t>
+  </si>
+  <si>
+    <t>368.00</t>
+  </si>
+  <si>
+    <t>680-831</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 남구 신정동 869-5 </t>
+  </si>
+  <si>
+    <t>울산광역시 남구 수암로 100 (신정동)</t>
+  </si>
+  <si>
+    <t>44748</t>
+  </si>
+  <si>
+    <t>서울국밥 수암점</t>
+  </si>
+  <si>
+    <t>2025-05-28 14:36:35</t>
+  </si>
+  <si>
+    <t>2025-05-30 02:40:00</t>
+  </si>
+  <si>
+    <t>11800</t>
+  </si>
+  <si>
+    <t>3700000-101-2001-00928</t>
+  </si>
+  <si>
+    <t>2001-10-12</t>
+  </si>
+  <si>
+    <t>052 2580027</t>
+  </si>
+  <si>
+    <t>194.46</t>
+  </si>
+  <si>
+    <t>680-817</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 남구 삼산동 1544-2 번지(지상1층) </t>
+  </si>
+  <si>
+    <t>울산광역시 남구 돋질로 322 (삼산동,번지(지상1층))</t>
+  </si>
+  <si>
+    <t>44713</t>
+  </si>
+  <si>
+    <t>투썸플레이스울산중리사거리점</t>
+  </si>
+  <si>
+    <t>2025-04-23 13:49:43</t>
+  </si>
+  <si>
+    <t>2025-04-25 02:40:00</t>
+  </si>
+  <si>
+    <t>11732</t>
+  </si>
+  <si>
+    <t>3700000-101-2006-00235</t>
+  </si>
+  <si>
+    <t>2006-07-12</t>
+  </si>
+  <si>
+    <t>052 2567444</t>
+  </si>
+  <si>
+    <t>55.25</t>
+  </si>
+  <si>
+    <t>680-804</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 남구 달동 972 번지(지하1층) </t>
+  </si>
+  <si>
+    <t>울산광역시 남구 삼산로 110 (달동,번지(지하1층))</t>
+  </si>
+  <si>
+    <t>44722</t>
+  </si>
+  <si>
+    <t>굿모닝병원장례식장</t>
+  </si>
+  <si>
+    <t>2023-09-08 10:50:23</t>
+  </si>
+  <si>
+    <t>2023-09-10 02:40:00</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>3690000-101-2024-00238</t>
+  </si>
+  <si>
+    <t>2024-12-20</t>
+  </si>
+  <si>
+    <t>2025-11-18</t>
+  </si>
+  <si>
+    <t>318.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 성안동 244 중구 문화의 전당 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 종가로 405, 중구 문화의 전당 3층 (성안동)</t>
+  </si>
+  <si>
+    <t>44543</t>
+  </si>
+  <si>
+    <t>컬쳐오공일</t>
+  </si>
+  <si>
+    <t>2025-11-18 09:23:14</t>
+  </si>
+  <si>
+    <t>2025-11-20 02:40:00</t>
+  </si>
+  <si>
+    <t>패밀리레스트랑</t>
+  </si>
+  <si>
+    <t>33396</t>
+  </si>
+  <si>
+    <t>3710000-101-2025-00007</t>
+  </si>
+  <si>
+    <t>2025-01-14</t>
+  </si>
+  <si>
+    <t>050713621201</t>
+  </si>
+  <si>
+    <t>90.78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 동구 방어동 69-5 </t>
+  </si>
+  <si>
+    <t>울산광역시 동구 등대4길 7, 1층 (방어동)</t>
+  </si>
+  <si>
+    <t>44059</t>
+  </si>
+  <si>
+    <t>술로밤 울산동구대왕암점</t>
+  </si>
+  <si>
+    <t>2025-05-07 15:21:08</t>
+  </si>
+  <si>
+    <t>2025-05-09 02:40:00</t>
+  </si>
+  <si>
+    <t>감성주점</t>
+  </si>
+  <si>
+    <t>33522</t>
+  </si>
+  <si>
+    <t>3710000-101-2025-00054</t>
+  </si>
+  <si>
+    <t>2025-04-16</t>
+  </si>
+  <si>
+    <t>65.47</t>
+  </si>
+  <si>
+    <t>682-814</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 동구 전하동 544-218 </t>
+  </si>
+  <si>
+    <t>울산광역시 동구 전하로 16, 1층 (전하동)</t>
+  </si>
+  <si>
+    <t>44039</t>
+  </si>
+  <si>
+    <t>빅대디포장마차 전하점</t>
+  </si>
+  <si>
+    <t>2025-05-20 17:36:39</t>
+  </si>
+  <si>
+    <t>2025-05-22 02:40:00</t>
+  </si>
+  <si>
+    <t>8093</t>
+  </si>
+  <si>
+    <t>3690000-101-2024-00231</t>
+  </si>
+  <si>
+    <t>2024-12-06</t>
+  </si>
+  <si>
+    <t>681-812</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 성남동 95-3 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 새즈믄해거리 6, 1층 (성남동)</t>
+  </si>
+  <si>
+    <t>44529</t>
+  </si>
+  <si>
+    <t>주효</t>
+  </si>
+  <si>
+    <t>2024-12-06 13:58:30</t>
+  </si>
+  <si>
+    <t>2024-12-08 00:11:52</t>
+  </si>
+  <si>
+    <t>경양식</t>
+  </si>
+  <si>
+    <t>8136</t>
+  </si>
+  <si>
+    <t>3690000-101-2022-00101</t>
+  </si>
+  <si>
+    <t>2022-06-15</t>
+  </si>
+  <si>
+    <t>72.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 옥교동 188-8 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 중앙길 171, 1층 (옥교동)</t>
+  </si>
+  <si>
+    <t>왓더버거 울산성남점</t>
+  </si>
+  <si>
+    <t>2024-02-19 15:20:09</t>
+  </si>
+  <si>
+    <t>2024-02-21 02:40:00</t>
+  </si>
+  <si>
+    <t>8137</t>
+  </si>
+  <si>
+    <t>3690000-101-2022-00103</t>
+  </si>
+  <si>
+    <t>71.76</t>
+  </si>
+  <si>
+    <t>681-310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 유곡동 478-7 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 종가2길 5-12, 1층 (유곡동)</t>
+  </si>
+  <si>
+    <t>44539</t>
+  </si>
+  <si>
+    <t>김선장초장집</t>
+  </si>
+  <si>
+    <t>2022-06-15 15:18:11</t>
+  </si>
+  <si>
+    <t>2022-06-18 00:22:31</t>
+  </si>
+  <si>
+    <t>횟집</t>
+  </si>
+  <si>
+    <t>8146</t>
+  </si>
+  <si>
+    <t>3690000-101-2022-00094</t>
+  </si>
+  <si>
+    <t>2022-06-07</t>
+  </si>
+  <si>
+    <t>052 245 0070</t>
+  </si>
+  <si>
+    <t>59.80</t>
+  </si>
+  <si>
+    <t>회뜨는김선장</t>
+  </si>
+  <si>
+    <t>2022-06-07 11:07:57</t>
+  </si>
+  <si>
+    <t>2022-06-09 00:22:31</t>
+  </si>
+  <si>
+    <t>8148</t>
+  </si>
+  <si>
+    <t>3690000-101-2022-00092</t>
+  </si>
+  <si>
+    <t>2022-06-02</t>
+  </si>
+  <si>
+    <t>70.74</t>
+  </si>
+  <si>
+    <t>681-816</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 우정동 385 선경아파트 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 우정3길 9, 상가동 2층 209호 (우정동, 선경아파트)</t>
+  </si>
+  <si>
+    <t>44464</t>
+  </si>
+  <si>
+    <t>양양양</t>
+  </si>
+  <si>
+    <t>2022-06-02 14:32:21</t>
+  </si>
+  <si>
+    <t>2022-06-04 00:22:32</t>
+  </si>
+  <si>
+    <t>8151</t>
+  </si>
+  <si>
+    <t>3690000-101-2022-00109</t>
+  </si>
+  <si>
+    <t>2022-06-24</t>
+  </si>
+  <si>
+    <t>41.53</t>
+  </si>
+  <si>
+    <t>681-822</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 학성동 354-1 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 새벽시장3길 10, 1층 (학성동)</t>
+  </si>
+  <si>
+    <t>44521</t>
+  </si>
+  <si>
+    <t>은이네 아나고집</t>
+  </si>
+  <si>
+    <t>2025-08-27 10:11:07</t>
+  </si>
+  <si>
+    <t>2025-08-29 02:40:00</t>
+  </si>
+  <si>
+    <t>8154</t>
+  </si>
+  <si>
+    <t>3690000-101-2022-00079</t>
+  </si>
+  <si>
+    <t>2022-05-10</t>
+  </si>
+  <si>
+    <t>154.22</t>
+  </si>
+  <si>
+    <t>681-420</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 장현동 156-2 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 종가25길 47, 1층 (장현동)</t>
+  </si>
+  <si>
+    <t>44548</t>
+  </si>
+  <si>
+    <t>해든쿠킹(haeden cooking)</t>
+  </si>
+  <si>
+    <t>2022-06-07 16:52:31</t>
+  </si>
+  <si>
+    <t>2022-06-09 02:40:00</t>
+  </si>
+  <si>
+    <t>8155</t>
+  </si>
+  <si>
+    <t>3690000-101-2022-00076</t>
+  </si>
+  <si>
+    <t>2022-04-28</t>
+  </si>
+  <si>
+    <t>50.00</t>
+  </si>
+  <si>
+    <t>681-220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 복산동 191-1 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 도화골5길 1, 1층 (복산동)</t>
+  </si>
+  <si>
+    <t>44477</t>
+  </si>
+  <si>
+    <t>요녀석중구점</t>
+  </si>
+  <si>
+    <t>2023-08-01 17:09:40</t>
+  </si>
+  <si>
+    <t>2023-08-03 02:40:00</t>
+  </si>
+  <si>
+    <t>8158</t>
+  </si>
+  <si>
+    <t>3690000-101-2023-00210</t>
+  </si>
+  <si>
+    <t>2023-11-03</t>
+  </si>
+  <si>
+    <t>113.62</t>
+  </si>
+  <si>
+    <t>681-818</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 태화동 22-26 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 유곡로 19, 2층 (태화동)</t>
+  </si>
+  <si>
+    <t>44452</t>
+  </si>
+  <si>
+    <t>하얼빈마라탕</t>
+  </si>
+  <si>
+    <t>2023-12-01 17:01:08</t>
+  </si>
+  <si>
+    <t>2023-12-03 02:40:00</t>
+  </si>
+  <si>
+    <t>8164</t>
+  </si>
+  <si>
+    <t>3690000-101-2023-00180</t>
+  </si>
+  <si>
+    <t>2023-09-21</t>
+  </si>
+  <si>
+    <t>183.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 옥교동 188-9 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 옥골샘8길 6, 1~2층 (옥교동)</t>
+  </si>
+  <si>
+    <t>판(paan)</t>
+  </si>
+  <si>
+    <t>2023-10-12 22:21:36</t>
+  </si>
+  <si>
+    <t>2023-10-14 02:40:00</t>
+  </si>
+  <si>
+    <t>8165</t>
+  </si>
+  <si>
+    <t>3690000-101-2023-00203</t>
+  </si>
+  <si>
+    <t>2023-10-27</t>
+  </si>
+  <si>
+    <t>39.90</t>
+  </si>
+  <si>
+    <t>681-240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 교동 294 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 동헌길 118, 1층 (교동)</t>
+  </si>
+  <si>
+    <t>44468</t>
+  </si>
+  <si>
+    <t>은이네아나고집</t>
+  </si>
+  <si>
+    <t>2023-11-27 20:10:46</t>
+  </si>
+  <si>
+    <t>2023-11-29 02:40:00</t>
+  </si>
+  <si>
+    <t>8171</t>
+  </si>
+  <si>
+    <t>3690000-101-2023-00181</t>
+  </si>
+  <si>
+    <t>2023-10-04</t>
+  </si>
+  <si>
+    <t>276.23</t>
+  </si>
+  <si>
+    <t>681-820</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 태화동 941-9 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 태화강국가정원길 23, 1~2층 (태화동)</t>
+  </si>
+  <si>
+    <t>44439</t>
+  </si>
+  <si>
+    <t>포이즈</t>
+  </si>
+  <si>
+    <t>2023-10-27 14:04:50</t>
+  </si>
+  <si>
+    <t>2023-10-29 02:40:00</t>
+  </si>
+  <si>
+    <t>8178</t>
+  </si>
+  <si>
+    <t>3690000-101-2023-00179</t>
+  </si>
+  <si>
+    <t>2023-09-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 서동 598-13 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 종가21길 47, 1층 (서동)</t>
+  </si>
+  <si>
+    <t>44547</t>
+  </si>
+  <si>
+    <t>파르메스</t>
+  </si>
+  <si>
+    <t>2023-09-20 16:14:33</t>
+  </si>
+  <si>
+    <t>2023-09-22 00:18:14</t>
+  </si>
+  <si>
+    <t>8183</t>
+  </si>
+  <si>
+    <t>3690000-101-2023-00225</t>
+  </si>
+  <si>
+    <t>2023-12-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 복산동 185-3 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 화합로 498, 1층 (복산동)</t>
+  </si>
+  <si>
+    <t>44475</t>
+  </si>
+  <si>
+    <t>마라장인마라탕중구점</t>
+  </si>
+  <si>
+    <t>2023-12-04 10:29:51</t>
+  </si>
+  <si>
+    <t>2023-12-06 00:17:03</t>
+  </si>
+  <si>
+    <t>8190</t>
+  </si>
+  <si>
+    <t>3690000-101-2025-00009</t>
+  </si>
+  <si>
+    <t>2025-01-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 태화동 471-18 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 신기1길 57, 1층 (태화동)</t>
+  </si>
+  <si>
+    <t>44456</t>
+  </si>
+  <si>
+    <t>빵심</t>
+  </si>
+  <si>
+    <t>2025-01-17 16:19:44</t>
+  </si>
+  <si>
+    <t>2025-01-19 00:11:35</t>
+  </si>
+  <si>
+    <t>8194</t>
+  </si>
+  <si>
+    <t>3690000-101-2024-00246</t>
+  </si>
+  <si>
+    <t>2024-12-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 복산동 472-6 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 계변고개 62, 1층 (복산동)</t>
+  </si>
+  <si>
+    <t>44470</t>
+  </si>
+  <si>
+    <t>서광회수산</t>
+  </si>
+  <si>
+    <t>2024-12-30 10:11:34</t>
+  </si>
+  <si>
+    <t>2025-01-01 00:11:33</t>
+  </si>
+  <si>
+    <t>8208</t>
+  </si>
+  <si>
+    <t>3690000-101-2018-00240</t>
+  </si>
+  <si>
+    <t>2018-11-15</t>
+  </si>
+  <si>
+    <t>052 285 0073</t>
+  </si>
+  <si>
+    <t>40.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 반구동 61-2 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 구교4길 14, 1층 일부 1호 (반구동)</t>
+  </si>
+  <si>
+    <t>푸줏간 울산중구점</t>
+  </si>
+  <si>
+    <t>2024-10-11 11:57:52</t>
+  </si>
+  <si>
+    <t>2024-10-13 02:40:00</t>
+  </si>
+  <si>
+    <t>9208</t>
+  </si>
+  <si>
+    <t>3690000-101-2009-00079</t>
+  </si>
+  <si>
+    <t>2009-05-19</t>
+  </si>
+  <si>
+    <t>070 88325585</t>
+  </si>
+  <si>
+    <t>102.96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 성남동 219-129 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 젊음의거리 40-3, 2층 (성남동)</t>
+  </si>
+  <si>
+    <t>44532</t>
+  </si>
+  <si>
+    <t>나마스까르(관광식당업)</t>
+  </si>
+  <si>
+    <t>2021-12-27 10:15:10</t>
+  </si>
+  <si>
+    <t>2021-12-29 02:40:00</t>
+  </si>
+  <si>
+    <t>9383</t>
+  </si>
+  <si>
+    <t>3690000-101-2014-00205</t>
+  </si>
+  <si>
+    <t>2014-11-14</t>
+  </si>
+  <si>
+    <t>052 245 8577</t>
+  </si>
+  <si>
+    <t>25.74</t>
+  </si>
+  <si>
+    <t>울산광역시 중구 유곡동 475-1번지 1층 106호</t>
+  </si>
+  <si>
+    <t>울산광역시 중구 종가4길 9, 1층 106호 (유곡동)</t>
+  </si>
+  <si>
+    <t>피자스쿨 유곡점</t>
+  </si>
+  <si>
+    <t>2016-12-14 13:51:46</t>
+  </si>
+  <si>
+    <t>9388</t>
+  </si>
+  <si>
+    <t>3690000-101-2014-00218</t>
+  </si>
+  <si>
+    <t>2014-12-03</t>
+  </si>
+  <si>
+    <t>052 275 8815</t>
+  </si>
+  <si>
+    <t>95.32</t>
+  </si>
+  <si>
+    <t>681-430</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 약사동 630-20 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 평산로 8 (약사동)</t>
+  </si>
+  <si>
+    <t>44472</t>
+  </si>
+  <si>
+    <t>남가족발</t>
+  </si>
+  <si>
+    <t>2024-12-02 14:55:02</t>
+  </si>
+  <si>
+    <t>2024-12-04 02:40:00</t>
+  </si>
+  <si>
+    <t>9743</t>
+  </si>
+  <si>
+    <t>3690000-101-2023-00031</t>
+  </si>
+  <si>
+    <t>2023-02-14</t>
+  </si>
+  <si>
+    <t>59.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 남외동 379-8 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 곽남6길 27, 1층 (남외동)</t>
+  </si>
+  <si>
+    <t>44491</t>
+  </si>
+  <si>
+    <t>베트남쌀국수</t>
+  </si>
+  <si>
+    <t>2023-02-14 16:23:53</t>
+  </si>
+  <si>
+    <t>2023-02-16 00:40:57</t>
+  </si>
+  <si>
+    <t>10489</t>
+  </si>
+  <si>
+    <t>3690000-101-2017-00098</t>
+  </si>
+  <si>
+    <t>2017-05-29</t>
+  </si>
+  <si>
+    <t>359.60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">울산광역시 중구 옥교동 95-14 </t>
+  </si>
+  <si>
+    <t>울산광역시 중구 젊음의거리 94, 2층 (옥교동)</t>
+  </si>
+  <si>
+    <t>후이&amp;뚜엔(HUY&amp;TUYEN)</t>
+  </si>
+  <si>
+    <t>2021-09-14 17:04:39</t>
+  </si>
+  <si>
+    <t>2021-09-16 02:40:00</t>
   </si>
 </sst>
 </file>
@@ -684,10 +1673,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -725,7 +1718,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -831,7 +1824,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -973,7 +1966,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -981,15 +1974,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8FD81BF-72DD-48DB-BA69-4E59C3FD3E0E}">
-  <dimension ref="A1:AU15"/>
+  <dimension ref="A1:AU46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AO17" sqref="AO17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB42" sqref="AB42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1069,7 +2062,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1149,7 +2142,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -1229,7 +2222,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -1309,7 +2302,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -1389,7 +2382,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>127</v>
       </c>
@@ -1469,7 +2462,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -1549,7 +2542,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>163</v>
       </c>
@@ -1662,7 +2655,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:47" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:47" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -1742,7 +2735,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>173</v>
       </c>
@@ -1831,7 +2824,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>97</v>
       </c>
@@ -1911,7 +2904,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -1991,7 +2984,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -2071,7 +3064,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -2160,7 +3153,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>153</v>
       </c>
@@ -2246,6 +3239,2765 @@
         <v>32</v>
       </c>
       <c r="AU15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>184</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>185</v>
+      </c>
+      <c r="E16" t="s">
+        <v>186</v>
+      </c>
+      <c r="F16" t="s">
+        <v>187</v>
+      </c>
+      <c r="G16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J16" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" t="s">
+        <v>35</v>
+      </c>
+      <c r="L16" t="s">
+        <v>32</v>
+      </c>
+      <c r="M16" t="s">
+        <v>32</v>
+      </c>
+      <c r="N16" t="s">
+        <v>32</v>
+      </c>
+      <c r="O16" t="s">
+        <v>32</v>
+      </c>
+      <c r="P16" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>189</v>
+      </c>
+      <c r="R16" t="s">
+        <v>190</v>
+      </c>
+      <c r="S16" t="s">
+        <v>191</v>
+      </c>
+      <c r="T16" t="s">
+        <v>192</v>
+      </c>
+      <c r="U16" t="s">
+        <v>193</v>
+      </c>
+      <c r="V16" t="s">
+        <v>194</v>
+      </c>
+      <c r="W16" t="s">
+        <v>195</v>
+      </c>
+      <c r="X16" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS16" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT16" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>185</v>
+      </c>
+      <c r="E17" t="s">
+        <v>198</v>
+      </c>
+      <c r="F17" t="s">
+        <v>199</v>
+      </c>
+      <c r="G17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17" t="s">
+        <v>32</v>
+      </c>
+      <c r="M17" t="s">
+        <v>32</v>
+      </c>
+      <c r="N17" t="s">
+        <v>32</v>
+      </c>
+      <c r="O17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P17" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>201</v>
+      </c>
+      <c r="R17" t="s">
+        <v>202</v>
+      </c>
+      <c r="S17" t="s">
+        <v>203</v>
+      </c>
+      <c r="T17" t="s">
+        <v>204</v>
+      </c>
+      <c r="U17" t="s">
+        <v>205</v>
+      </c>
+      <c r="V17" t="s">
+        <v>206</v>
+      </c>
+      <c r="W17" t="s">
+        <v>207</v>
+      </c>
+      <c r="X17" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>208</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>185</v>
+      </c>
+      <c r="E18" t="s">
+        <v>209</v>
+      </c>
+      <c r="F18" t="s">
+        <v>210</v>
+      </c>
+      <c r="G18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18" t="s">
+        <v>35</v>
+      </c>
+      <c r="L18" t="s">
+        <v>32</v>
+      </c>
+      <c r="M18" t="s">
+        <v>32</v>
+      </c>
+      <c r="N18" t="s">
+        <v>32</v>
+      </c>
+      <c r="O18" t="s">
+        <v>32</v>
+      </c>
+      <c r="P18" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>212</v>
+      </c>
+      <c r="R18" t="s">
+        <v>213</v>
+      </c>
+      <c r="S18" t="s">
+        <v>214</v>
+      </c>
+      <c r="T18" t="s">
+        <v>215</v>
+      </c>
+      <c r="U18" t="s">
+        <v>216</v>
+      </c>
+      <c r="V18" t="s">
+        <v>217</v>
+      </c>
+      <c r="W18" t="s">
+        <v>218</v>
+      </c>
+      <c r="X18" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>219</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS18" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT18" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>220</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>185</v>
+      </c>
+      <c r="E19" t="s">
+        <v>221</v>
+      </c>
+      <c r="F19" t="s">
+        <v>222</v>
+      </c>
+      <c r="G19" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" t="s">
+        <v>34</v>
+      </c>
+      <c r="J19" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19" t="s">
+        <v>35</v>
+      </c>
+      <c r="L19" t="s">
+        <v>32</v>
+      </c>
+      <c r="M19" t="s">
+        <v>32</v>
+      </c>
+      <c r="N19" t="s">
+        <v>32</v>
+      </c>
+      <c r="O19" t="s">
+        <v>32</v>
+      </c>
+      <c r="P19" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>224</v>
+      </c>
+      <c r="R19" t="s">
+        <v>225</v>
+      </c>
+      <c r="S19" t="s">
+        <v>226</v>
+      </c>
+      <c r="T19" t="s">
+        <v>227</v>
+      </c>
+      <c r="U19" t="s">
+        <v>228</v>
+      </c>
+      <c r="V19" t="s">
+        <v>229</v>
+      </c>
+      <c r="W19" t="s">
+        <v>230</v>
+      </c>
+      <c r="X19" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>231</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS19" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT19" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>232</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>185</v>
+      </c>
+      <c r="E20" t="s">
+        <v>233</v>
+      </c>
+      <c r="F20" t="s">
+        <v>234</v>
+      </c>
+      <c r="G20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" t="s">
+        <v>34</v>
+      </c>
+      <c r="J20" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" t="s">
+        <v>32</v>
+      </c>
+      <c r="M20" t="s">
+        <v>32</v>
+      </c>
+      <c r="N20" t="s">
+        <v>32</v>
+      </c>
+      <c r="O20" t="s">
+        <v>32</v>
+      </c>
+      <c r="P20" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>236</v>
+      </c>
+      <c r="R20" t="s">
+        <v>237</v>
+      </c>
+      <c r="S20" t="s">
+        <v>238</v>
+      </c>
+      <c r="T20" t="s">
+        <v>239</v>
+      </c>
+      <c r="U20" t="s">
+        <v>240</v>
+      </c>
+      <c r="V20" t="s">
+        <v>241</v>
+      </c>
+      <c r="W20" t="s">
+        <v>242</v>
+      </c>
+      <c r="X20" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>243</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS20" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT20" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>244</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
+        <v>185</v>
+      </c>
+      <c r="E21" t="s">
+        <v>245</v>
+      </c>
+      <c r="F21" t="s">
+        <v>246</v>
+      </c>
+      <c r="G21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" t="s">
+        <v>33</v>
+      </c>
+      <c r="K21" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" t="s">
+        <v>32</v>
+      </c>
+      <c r="M21" t="s">
+        <v>32</v>
+      </c>
+      <c r="N21" t="s">
+        <v>32</v>
+      </c>
+      <c r="O21" t="s">
+        <v>32</v>
+      </c>
+      <c r="P21" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>248</v>
+      </c>
+      <c r="R21" t="s">
+        <v>249</v>
+      </c>
+      <c r="S21" t="s">
+        <v>250</v>
+      </c>
+      <c r="T21" t="s">
+        <v>251</v>
+      </c>
+      <c r="U21" t="s">
+        <v>252</v>
+      </c>
+      <c r="V21" t="s">
+        <v>253</v>
+      </c>
+      <c r="W21" t="s">
+        <v>254</v>
+      </c>
+      <c r="X21" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>255</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS21" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT21" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>256</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" t="s">
+        <v>257</v>
+      </c>
+      <c r="F22" t="s">
+        <v>258</v>
+      </c>
+      <c r="G22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" t="s">
+        <v>130</v>
+      </c>
+      <c r="I22" t="s">
+        <v>131</v>
+      </c>
+      <c r="J22" t="s">
+        <v>132</v>
+      </c>
+      <c r="K22" t="s">
+        <v>131</v>
+      </c>
+      <c r="L22" t="s">
+        <v>259</v>
+      </c>
+      <c r="M22" t="s">
+        <v>32</v>
+      </c>
+      <c r="N22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O22" t="s">
+        <v>32</v>
+      </c>
+      <c r="P22" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>260</v>
+      </c>
+      <c r="R22" t="s">
+        <v>120</v>
+      </c>
+      <c r="S22" t="s">
+        <v>261</v>
+      </c>
+      <c r="T22" t="s">
+        <v>262</v>
+      </c>
+      <c r="U22" t="s">
+        <v>263</v>
+      </c>
+      <c r="V22" t="s">
+        <v>264</v>
+      </c>
+      <c r="W22" t="s">
+        <v>265</v>
+      </c>
+      <c r="X22" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>266</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>267</v>
+      </c>
+      <c r="AS22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>268</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" t="s">
+        <v>269</v>
+      </c>
+      <c r="F23" t="s">
+        <v>270</v>
+      </c>
+      <c r="G23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" t="s">
+        <v>34</v>
+      </c>
+      <c r="J23" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23" t="s">
+        <v>32</v>
+      </c>
+      <c r="M23" t="s">
+        <v>32</v>
+      </c>
+      <c r="N23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O23" t="s">
+        <v>32</v>
+      </c>
+      <c r="P23" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>272</v>
+      </c>
+      <c r="R23" t="s">
+        <v>159</v>
+      </c>
+      <c r="S23" t="s">
+        <v>273</v>
+      </c>
+      <c r="T23" t="s">
+        <v>274</v>
+      </c>
+      <c r="U23" t="s">
+        <v>275</v>
+      </c>
+      <c r="V23" t="s">
+        <v>276</v>
+      </c>
+      <c r="W23" t="s">
+        <v>277</v>
+      </c>
+      <c r="X23" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>278</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>279</v>
+      </c>
+      <c r="AS23" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT23" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>280</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s">
+        <v>143</v>
+      </c>
+      <c r="E24" t="s">
+        <v>281</v>
+      </c>
+      <c r="F24" t="s">
+        <v>282</v>
+      </c>
+      <c r="G24" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J24" t="s">
+        <v>33</v>
+      </c>
+      <c r="K24" t="s">
+        <v>35</v>
+      </c>
+      <c r="L24" t="s">
+        <v>32</v>
+      </c>
+      <c r="M24" t="s">
+        <v>32</v>
+      </c>
+      <c r="N24" t="s">
+        <v>32</v>
+      </c>
+      <c r="O24" t="s">
+        <v>32</v>
+      </c>
+      <c r="P24" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>283</v>
+      </c>
+      <c r="R24" t="s">
+        <v>284</v>
+      </c>
+      <c r="S24" t="s">
+        <v>285</v>
+      </c>
+      <c r="T24" t="s">
+        <v>286</v>
+      </c>
+      <c r="U24" t="s">
+        <v>287</v>
+      </c>
+      <c r="V24" t="s">
+        <v>288</v>
+      </c>
+      <c r="W24" t="s">
+        <v>289</v>
+      </c>
+      <c r="X24" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>290</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>279</v>
+      </c>
+      <c r="AS24" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT24" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>291</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" t="s">
+        <v>292</v>
+      </c>
+      <c r="F25" t="s">
+        <v>293</v>
+      </c>
+      <c r="G25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" t="s">
+        <v>34</v>
+      </c>
+      <c r="J25" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" t="s">
+        <v>35</v>
+      </c>
+      <c r="L25" t="s">
+        <v>32</v>
+      </c>
+      <c r="M25" t="s">
+        <v>32</v>
+      </c>
+      <c r="N25" t="s">
+        <v>32</v>
+      </c>
+      <c r="O25" t="s">
+        <v>32</v>
+      </c>
+      <c r="P25" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>36</v>
+      </c>
+      <c r="R25" t="s">
+        <v>294</v>
+      </c>
+      <c r="S25" t="s">
+        <v>295</v>
+      </c>
+      <c r="T25" t="s">
+        <v>296</v>
+      </c>
+      <c r="U25" t="s">
+        <v>297</v>
+      </c>
+      <c r="V25" t="s">
+        <v>298</v>
+      </c>
+      <c r="W25" t="s">
+        <v>299</v>
+      </c>
+      <c r="X25" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>300</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>301</v>
+      </c>
+      <c r="AS25" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT25" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>302</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" t="s">
+        <v>303</v>
+      </c>
+      <c r="F26" t="s">
+        <v>304</v>
+      </c>
+      <c r="G26" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I26" t="s">
+        <v>34</v>
+      </c>
+      <c r="J26" t="s">
+        <v>33</v>
+      </c>
+      <c r="K26" t="s">
+        <v>35</v>
+      </c>
+      <c r="L26" t="s">
+        <v>32</v>
+      </c>
+      <c r="M26" t="s">
+        <v>32</v>
+      </c>
+      <c r="N26" t="s">
+        <v>32</v>
+      </c>
+      <c r="O26" t="s">
+        <v>32</v>
+      </c>
+      <c r="P26" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>305</v>
+      </c>
+      <c r="R26" t="s">
+        <v>50</v>
+      </c>
+      <c r="S26" t="s">
+        <v>306</v>
+      </c>
+      <c r="T26" t="s">
+        <v>307</v>
+      </c>
+      <c r="U26" t="s">
+        <v>53</v>
+      </c>
+      <c r="V26" t="s">
+        <v>308</v>
+      </c>
+      <c r="W26" t="s">
+        <v>309</v>
+      </c>
+      <c r="X26" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>310</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>301</v>
+      </c>
+      <c r="AS26" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT26" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>311</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" t="s">
+        <v>312</v>
+      </c>
+      <c r="F27" t="s">
+        <v>304</v>
+      </c>
+      <c r="G27" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" t="s">
+        <v>33</v>
+      </c>
+      <c r="I27" t="s">
+        <v>34</v>
+      </c>
+      <c r="J27" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27" t="s">
+        <v>35</v>
+      </c>
+      <c r="L27" t="s">
+        <v>32</v>
+      </c>
+      <c r="M27" t="s">
+        <v>32</v>
+      </c>
+      <c r="N27" t="s">
+        <v>32</v>
+      </c>
+      <c r="O27" t="s">
+        <v>32</v>
+      </c>
+      <c r="P27" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>313</v>
+      </c>
+      <c r="R27" t="s">
+        <v>314</v>
+      </c>
+      <c r="S27" t="s">
+        <v>315</v>
+      </c>
+      <c r="T27" t="s">
+        <v>316</v>
+      </c>
+      <c r="U27" t="s">
+        <v>317</v>
+      </c>
+      <c r="V27" t="s">
+        <v>318</v>
+      </c>
+      <c r="W27" t="s">
+        <v>319</v>
+      </c>
+      <c r="X27" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>320</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>321</v>
+      </c>
+      <c r="AS27" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT27" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>322</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" t="s">
+        <v>323</v>
+      </c>
+      <c r="F28" t="s">
+        <v>324</v>
+      </c>
+      <c r="G28" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" t="s">
+        <v>34</v>
+      </c>
+      <c r="J28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28" t="s">
+        <v>35</v>
+      </c>
+      <c r="L28" t="s">
+        <v>32</v>
+      </c>
+      <c r="M28" t="s">
+        <v>32</v>
+      </c>
+      <c r="N28" t="s">
+        <v>32</v>
+      </c>
+      <c r="O28" t="s">
+        <v>32</v>
+      </c>
+      <c r="P28" t="s">
+        <v>325</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>326</v>
+      </c>
+      <c r="R28" t="s">
+        <v>314</v>
+      </c>
+      <c r="S28" t="s">
+        <v>315</v>
+      </c>
+      <c r="T28" t="s">
+        <v>316</v>
+      </c>
+      <c r="U28" t="s">
+        <v>317</v>
+      </c>
+      <c r="V28" t="s">
+        <v>327</v>
+      </c>
+      <c r="W28" t="s">
+        <v>328</v>
+      </c>
+      <c r="X28" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>329</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>321</v>
+      </c>
+      <c r="AS28" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT28" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>330</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" t="s">
+        <v>331</v>
+      </c>
+      <c r="F29" t="s">
+        <v>332</v>
+      </c>
+      <c r="G29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" t="s">
+        <v>34</v>
+      </c>
+      <c r="J29" t="s">
+        <v>33</v>
+      </c>
+      <c r="K29" t="s">
+        <v>35</v>
+      </c>
+      <c r="L29" t="s">
+        <v>32</v>
+      </c>
+      <c r="M29" t="s">
+        <v>32</v>
+      </c>
+      <c r="N29" t="s">
+        <v>32</v>
+      </c>
+      <c r="O29" t="s">
+        <v>32</v>
+      </c>
+      <c r="P29" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>333</v>
+      </c>
+      <c r="R29" t="s">
+        <v>334</v>
+      </c>
+      <c r="S29" t="s">
+        <v>335</v>
+      </c>
+      <c r="T29" t="s">
+        <v>336</v>
+      </c>
+      <c r="U29" t="s">
+        <v>337</v>
+      </c>
+      <c r="V29" t="s">
+        <v>338</v>
+      </c>
+      <c r="W29" t="s">
+        <v>339</v>
+      </c>
+      <c r="X29" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>340</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS29" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT29" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>341</v>
+      </c>
+      <c r="B30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" t="s">
+        <v>342</v>
+      </c>
+      <c r="F30" t="s">
+        <v>343</v>
+      </c>
+      <c r="G30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" t="s">
+        <v>33</v>
+      </c>
+      <c r="I30" t="s">
+        <v>34</v>
+      </c>
+      <c r="J30" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" t="s">
+        <v>35</v>
+      </c>
+      <c r="L30" t="s">
+        <v>32</v>
+      </c>
+      <c r="M30" t="s">
+        <v>32</v>
+      </c>
+      <c r="N30" t="s">
+        <v>32</v>
+      </c>
+      <c r="O30" t="s">
+        <v>32</v>
+      </c>
+      <c r="P30" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>344</v>
+      </c>
+      <c r="R30" t="s">
+        <v>345</v>
+      </c>
+      <c r="S30" t="s">
+        <v>346</v>
+      </c>
+      <c r="T30" t="s">
+        <v>347</v>
+      </c>
+      <c r="U30" t="s">
+        <v>348</v>
+      </c>
+      <c r="V30" t="s">
+        <v>349</v>
+      </c>
+      <c r="W30" t="s">
+        <v>350</v>
+      </c>
+      <c r="X30" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>351</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>321</v>
+      </c>
+      <c r="AS30" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT30" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>352</v>
+      </c>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" t="s">
+        <v>353</v>
+      </c>
+      <c r="F31" t="s">
+        <v>354</v>
+      </c>
+      <c r="G31" t="s">
+        <v>32</v>
+      </c>
+      <c r="H31" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" t="s">
+        <v>34</v>
+      </c>
+      <c r="J31" t="s">
+        <v>33</v>
+      </c>
+      <c r="K31" t="s">
+        <v>35</v>
+      </c>
+      <c r="L31" t="s">
+        <v>32</v>
+      </c>
+      <c r="M31" t="s">
+        <v>32</v>
+      </c>
+      <c r="N31" t="s">
+        <v>32</v>
+      </c>
+      <c r="O31" t="s">
+        <v>32</v>
+      </c>
+      <c r="P31" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>355</v>
+      </c>
+      <c r="R31" t="s">
+        <v>356</v>
+      </c>
+      <c r="S31" t="s">
+        <v>357</v>
+      </c>
+      <c r="T31" t="s">
+        <v>358</v>
+      </c>
+      <c r="U31" t="s">
+        <v>359</v>
+      </c>
+      <c r="V31" t="s">
+        <v>360</v>
+      </c>
+      <c r="W31" t="s">
+        <v>361</v>
+      </c>
+      <c r="X31" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>362</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>267</v>
+      </c>
+      <c r="AS31" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT31" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>363</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" t="s">
+        <v>364</v>
+      </c>
+      <c r="F32" t="s">
+        <v>365</v>
+      </c>
+      <c r="G32" t="s">
+        <v>32</v>
+      </c>
+      <c r="H32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" t="s">
+        <v>35</v>
+      </c>
+      <c r="L32" t="s">
+        <v>32</v>
+      </c>
+      <c r="M32" t="s">
+        <v>32</v>
+      </c>
+      <c r="N32" t="s">
+        <v>32</v>
+      </c>
+      <c r="O32" t="s">
+        <v>32</v>
+      </c>
+      <c r="P32" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>366</v>
+      </c>
+      <c r="R32" t="s">
+        <v>367</v>
+      </c>
+      <c r="S32" t="s">
+        <v>368</v>
+      </c>
+      <c r="T32" t="s">
+        <v>369</v>
+      </c>
+      <c r="U32" t="s">
+        <v>370</v>
+      </c>
+      <c r="V32" t="s">
+        <v>371</v>
+      </c>
+      <c r="W32" t="s">
+        <v>372</v>
+      </c>
+      <c r="X32" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>373</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>267</v>
+      </c>
+      <c r="AS32" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT32" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>374</v>
+      </c>
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" t="s">
+        <v>375</v>
+      </c>
+      <c r="F33" t="s">
+        <v>376</v>
+      </c>
+      <c r="G33" t="s">
+        <v>32</v>
+      </c>
+      <c r="H33" t="s">
+        <v>33</v>
+      </c>
+      <c r="I33" t="s">
+        <v>34</v>
+      </c>
+      <c r="J33" t="s">
+        <v>33</v>
+      </c>
+      <c r="K33" t="s">
+        <v>35</v>
+      </c>
+      <c r="L33" t="s">
+        <v>32</v>
+      </c>
+      <c r="M33" t="s">
+        <v>32</v>
+      </c>
+      <c r="N33" t="s">
+        <v>32</v>
+      </c>
+      <c r="O33" t="s">
+        <v>32</v>
+      </c>
+      <c r="P33" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>377</v>
+      </c>
+      <c r="R33" t="s">
+        <v>378</v>
+      </c>
+      <c r="S33" t="s">
+        <v>379</v>
+      </c>
+      <c r="T33" t="s">
+        <v>380</v>
+      </c>
+      <c r="U33" t="s">
+        <v>381</v>
+      </c>
+      <c r="V33" t="s">
+        <v>382</v>
+      </c>
+      <c r="W33" t="s">
+        <v>383</v>
+      </c>
+      <c r="X33" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>384</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS33" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT33" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>385</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" t="s">
+        <v>386</v>
+      </c>
+      <c r="F34" t="s">
+        <v>387</v>
+      </c>
+      <c r="G34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H34" t="s">
+        <v>33</v>
+      </c>
+      <c r="I34" t="s">
+        <v>34</v>
+      </c>
+      <c r="J34" t="s">
+        <v>33</v>
+      </c>
+      <c r="K34" t="s">
+        <v>35</v>
+      </c>
+      <c r="L34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N34" t="s">
+        <v>32</v>
+      </c>
+      <c r="O34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P34" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>388</v>
+      </c>
+      <c r="R34" t="s">
+        <v>50</v>
+      </c>
+      <c r="S34" t="s">
+        <v>389</v>
+      </c>
+      <c r="T34" t="s">
+        <v>390</v>
+      </c>
+      <c r="U34" t="s">
+        <v>53</v>
+      </c>
+      <c r="V34" t="s">
+        <v>391</v>
+      </c>
+      <c r="W34" t="s">
+        <v>392</v>
+      </c>
+      <c r="X34" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>393</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>301</v>
+      </c>
+      <c r="AS34" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT34" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>394</v>
+      </c>
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" t="s">
+        <v>395</v>
+      </c>
+      <c r="F35" t="s">
+        <v>396</v>
+      </c>
+      <c r="G35" t="s">
+        <v>32</v>
+      </c>
+      <c r="H35" t="s">
+        <v>33</v>
+      </c>
+      <c r="I35" t="s">
+        <v>34</v>
+      </c>
+      <c r="J35" t="s">
+        <v>33</v>
+      </c>
+      <c r="K35" t="s">
+        <v>35</v>
+      </c>
+      <c r="L35" t="s">
+        <v>32</v>
+      </c>
+      <c r="M35" t="s">
+        <v>32</v>
+      </c>
+      <c r="N35" t="s">
+        <v>32</v>
+      </c>
+      <c r="O35" t="s">
+        <v>32</v>
+      </c>
+      <c r="P35" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>397</v>
+      </c>
+      <c r="R35" t="s">
+        <v>398</v>
+      </c>
+      <c r="S35" t="s">
+        <v>399</v>
+      </c>
+      <c r="T35" t="s">
+        <v>400</v>
+      </c>
+      <c r="U35" t="s">
+        <v>401</v>
+      </c>
+      <c r="V35" t="s">
+        <v>402</v>
+      </c>
+      <c r="W35" t="s">
+        <v>403</v>
+      </c>
+      <c r="X35" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>404</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>321</v>
+      </c>
+      <c r="AS35" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT35" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>405</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" t="s">
+        <v>406</v>
+      </c>
+      <c r="F36" t="s">
+        <v>407</v>
+      </c>
+      <c r="G36" t="s">
+        <v>32</v>
+      </c>
+      <c r="H36" t="s">
+        <v>33</v>
+      </c>
+      <c r="I36" t="s">
+        <v>34</v>
+      </c>
+      <c r="J36" t="s">
+        <v>33</v>
+      </c>
+      <c r="K36" t="s">
+        <v>35</v>
+      </c>
+      <c r="L36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M36" t="s">
+        <v>32</v>
+      </c>
+      <c r="N36" t="s">
+        <v>32</v>
+      </c>
+      <c r="O36" t="s">
+        <v>32</v>
+      </c>
+      <c r="P36" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>408</v>
+      </c>
+      <c r="R36" t="s">
+        <v>409</v>
+      </c>
+      <c r="S36" t="s">
+        <v>410</v>
+      </c>
+      <c r="T36" t="s">
+        <v>411</v>
+      </c>
+      <c r="U36" t="s">
+        <v>412</v>
+      </c>
+      <c r="V36" t="s">
+        <v>413</v>
+      </c>
+      <c r="W36" t="s">
+        <v>414</v>
+      </c>
+      <c r="X36" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>415</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>301</v>
+      </c>
+      <c r="AS36" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT36" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>416</v>
+      </c>
+      <c r="B37" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" t="s">
+        <v>417</v>
+      </c>
+      <c r="F37" t="s">
+        <v>418</v>
+      </c>
+      <c r="G37" t="s">
+        <v>32</v>
+      </c>
+      <c r="H37" t="s">
+        <v>33</v>
+      </c>
+      <c r="I37" t="s">
+        <v>34</v>
+      </c>
+      <c r="J37" t="s">
+        <v>33</v>
+      </c>
+      <c r="K37" t="s">
+        <v>35</v>
+      </c>
+      <c r="L37" t="s">
+        <v>32</v>
+      </c>
+      <c r="M37" t="s">
+        <v>32</v>
+      </c>
+      <c r="N37" t="s">
+        <v>32</v>
+      </c>
+      <c r="O37" t="s">
+        <v>32</v>
+      </c>
+      <c r="P37" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>36</v>
+      </c>
+      <c r="R37" t="s">
+        <v>90</v>
+      </c>
+      <c r="S37" t="s">
+        <v>419</v>
+      </c>
+      <c r="T37" t="s">
+        <v>420</v>
+      </c>
+      <c r="U37" t="s">
+        <v>421</v>
+      </c>
+      <c r="V37" t="s">
+        <v>422</v>
+      </c>
+      <c r="W37" t="s">
+        <v>423</v>
+      </c>
+      <c r="X37" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>424</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>301</v>
+      </c>
+      <c r="AS37" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT37" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>425</v>
+      </c>
+      <c r="B38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" t="s">
+        <v>426</v>
+      </c>
+      <c r="F38" t="s">
+        <v>427</v>
+      </c>
+      <c r="G38" t="s">
+        <v>32</v>
+      </c>
+      <c r="H38" t="s">
+        <v>33</v>
+      </c>
+      <c r="I38" t="s">
+        <v>34</v>
+      </c>
+      <c r="J38" t="s">
+        <v>33</v>
+      </c>
+      <c r="K38" t="s">
+        <v>35</v>
+      </c>
+      <c r="L38" t="s">
+        <v>32</v>
+      </c>
+      <c r="M38" t="s">
+        <v>32</v>
+      </c>
+      <c r="N38" t="s">
+        <v>32</v>
+      </c>
+      <c r="O38" t="s">
+        <v>32</v>
+      </c>
+      <c r="P38" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>32</v>
+      </c>
+      <c r="R38" t="s">
+        <v>367</v>
+      </c>
+      <c r="S38" t="s">
+        <v>428</v>
+      </c>
+      <c r="T38" t="s">
+        <v>429</v>
+      </c>
+      <c r="U38" t="s">
+        <v>430</v>
+      </c>
+      <c r="V38" t="s">
+        <v>431</v>
+      </c>
+      <c r="W38" t="s">
+        <v>432</v>
+      </c>
+      <c r="X38" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>433</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS38" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT38" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>434</v>
+      </c>
+      <c r="B39" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" t="s">
+        <v>435</v>
+      </c>
+      <c r="F39" t="s">
+        <v>436</v>
+      </c>
+      <c r="G39" t="s">
+        <v>32</v>
+      </c>
+      <c r="H39" t="s">
+        <v>33</v>
+      </c>
+      <c r="I39" t="s">
+        <v>34</v>
+      </c>
+      <c r="J39" t="s">
+        <v>33</v>
+      </c>
+      <c r="K39" t="s">
+        <v>35</v>
+      </c>
+      <c r="L39" t="s">
+        <v>32</v>
+      </c>
+      <c r="M39" t="s">
+        <v>32</v>
+      </c>
+      <c r="N39" t="s">
+        <v>32</v>
+      </c>
+      <c r="O39" t="s">
+        <v>32</v>
+      </c>
+      <c r="P39" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>32</v>
+      </c>
+      <c r="R39" t="s">
+        <v>100</v>
+      </c>
+      <c r="S39" t="s">
+        <v>437</v>
+      </c>
+      <c r="T39" t="s">
+        <v>438</v>
+      </c>
+      <c r="U39" t="s">
+        <v>439</v>
+      </c>
+      <c r="V39" t="s">
+        <v>440</v>
+      </c>
+      <c r="W39" t="s">
+        <v>441</v>
+      </c>
+      <c r="X39" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>442</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>301</v>
+      </c>
+      <c r="AS39" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT39" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>443</v>
+      </c>
+      <c r="B40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" t="s">
+        <v>444</v>
+      </c>
+      <c r="F40" t="s">
+        <v>445</v>
+      </c>
+      <c r="G40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H40" t="s">
+        <v>33</v>
+      </c>
+      <c r="I40" t="s">
+        <v>34</v>
+      </c>
+      <c r="J40" t="s">
+        <v>33</v>
+      </c>
+      <c r="K40" t="s">
+        <v>35</v>
+      </c>
+      <c r="L40" t="s">
+        <v>32</v>
+      </c>
+      <c r="M40" t="s">
+        <v>32</v>
+      </c>
+      <c r="N40" t="s">
+        <v>32</v>
+      </c>
+      <c r="O40" t="s">
+        <v>32</v>
+      </c>
+      <c r="P40" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>32</v>
+      </c>
+      <c r="R40" t="s">
+        <v>367</v>
+      </c>
+      <c r="S40" t="s">
+        <v>446</v>
+      </c>
+      <c r="T40" t="s">
+        <v>447</v>
+      </c>
+      <c r="U40" t="s">
+        <v>448</v>
+      </c>
+      <c r="V40" t="s">
+        <v>449</v>
+      </c>
+      <c r="W40" t="s">
+        <v>450</v>
+      </c>
+      <c r="X40" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>451</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>321</v>
+      </c>
+      <c r="AS40" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT40" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>452</v>
+      </c>
+      <c r="B41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" t="s">
+        <v>453</v>
+      </c>
+      <c r="F41" t="s">
+        <v>454</v>
+      </c>
+      <c r="G41" t="s">
+        <v>32</v>
+      </c>
+      <c r="H41" t="s">
+        <v>33</v>
+      </c>
+      <c r="I41" t="s">
+        <v>34</v>
+      </c>
+      <c r="J41" t="s">
+        <v>33</v>
+      </c>
+      <c r="K41" t="s">
+        <v>35</v>
+      </c>
+      <c r="L41" t="s">
+        <v>32</v>
+      </c>
+      <c r="M41" t="s">
+        <v>32</v>
+      </c>
+      <c r="N41" t="s">
+        <v>32</v>
+      </c>
+      <c r="O41" t="s">
+        <v>32</v>
+      </c>
+      <c r="P41" t="s">
+        <v>455</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>456</v>
+      </c>
+      <c r="R41" t="s">
+        <v>62</v>
+      </c>
+      <c r="S41" t="s">
+        <v>457</v>
+      </c>
+      <c r="T41" t="s">
+        <v>458</v>
+      </c>
+      <c r="U41" t="s">
+        <v>65</v>
+      </c>
+      <c r="V41" t="s">
+        <v>459</v>
+      </c>
+      <c r="W41" t="s">
+        <v>460</v>
+      </c>
+      <c r="X41" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>461</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>301</v>
+      </c>
+      <c r="AS41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT41" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>462</v>
+      </c>
+      <c r="B42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" t="s">
+        <v>463</v>
+      </c>
+      <c r="F42" t="s">
+        <v>464</v>
+      </c>
+      <c r="G42" t="s">
+        <v>32</v>
+      </c>
+      <c r="H42" t="s">
+        <v>33</v>
+      </c>
+      <c r="I42" t="s">
+        <v>34</v>
+      </c>
+      <c r="J42" t="s">
+        <v>33</v>
+      </c>
+      <c r="K42" t="s">
+        <v>35</v>
+      </c>
+      <c r="L42" t="s">
+        <v>32</v>
+      </c>
+      <c r="M42" t="s">
+        <v>32</v>
+      </c>
+      <c r="N42" t="s">
+        <v>32</v>
+      </c>
+      <c r="O42" t="s">
+        <v>32</v>
+      </c>
+      <c r="P42" t="s">
+        <v>465</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>466</v>
+      </c>
+      <c r="R42" t="s">
+        <v>294</v>
+      </c>
+      <c r="S42" t="s">
+        <v>467</v>
+      </c>
+      <c r="T42" t="s">
+        <v>468</v>
+      </c>
+      <c r="U42" t="s">
+        <v>469</v>
+      </c>
+      <c r="V42" t="s">
+        <v>470</v>
+      </c>
+      <c r="W42" t="s">
+        <v>471</v>
+      </c>
+      <c r="X42" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>472</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>78</v>
+      </c>
+      <c r="AS42" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT42" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU42" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>473</v>
+      </c>
+      <c r="B43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E43" t="s">
+        <v>474</v>
+      </c>
+      <c r="F43" t="s">
+        <v>475</v>
+      </c>
+      <c r="G43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H43" t="s">
+        <v>33</v>
+      </c>
+      <c r="I43" t="s">
+        <v>34</v>
+      </c>
+      <c r="J43" t="s">
+        <v>33</v>
+      </c>
+      <c r="K43" t="s">
+        <v>35</v>
+      </c>
+      <c r="L43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N43" t="s">
+        <v>32</v>
+      </c>
+      <c r="O43" t="s">
+        <v>32</v>
+      </c>
+      <c r="P43" t="s">
+        <v>476</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>477</v>
+      </c>
+      <c r="R43" t="s">
+        <v>314</v>
+      </c>
+      <c r="S43" t="s">
+        <v>478</v>
+      </c>
+      <c r="T43" t="s">
+        <v>479</v>
+      </c>
+      <c r="U43" t="s">
+        <v>317</v>
+      </c>
+      <c r="V43" t="s">
+        <v>480</v>
+      </c>
+      <c r="W43" t="s">
+        <v>481</v>
+      </c>
+      <c r="X43" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>78</v>
+      </c>
+      <c r="AS43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>482</v>
+      </c>
+      <c r="B44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" t="s">
+        <v>483</v>
+      </c>
+      <c r="F44" t="s">
+        <v>484</v>
+      </c>
+      <c r="G44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H44" t="s">
+        <v>33</v>
+      </c>
+      <c r="I44" t="s">
+        <v>34</v>
+      </c>
+      <c r="J44" t="s">
+        <v>33</v>
+      </c>
+      <c r="K44" t="s">
+        <v>35</v>
+      </c>
+      <c r="L44" t="s">
+        <v>32</v>
+      </c>
+      <c r="M44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N44" t="s">
+        <v>32</v>
+      </c>
+      <c r="O44" t="s">
+        <v>32</v>
+      </c>
+      <c r="P44" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>486</v>
+      </c>
+      <c r="R44" t="s">
+        <v>487</v>
+      </c>
+      <c r="S44" t="s">
+        <v>488</v>
+      </c>
+      <c r="T44" t="s">
+        <v>489</v>
+      </c>
+      <c r="U44" t="s">
+        <v>490</v>
+      </c>
+      <c r="V44" t="s">
+        <v>491</v>
+      </c>
+      <c r="W44" t="s">
+        <v>492</v>
+      </c>
+      <c r="X44" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>493</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>107</v>
+      </c>
+      <c r="AS44" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT44" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>494</v>
+      </c>
+      <c r="B45" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" t="s">
+        <v>29</v>
+      </c>
+      <c r="E45" t="s">
+        <v>495</v>
+      </c>
+      <c r="F45" t="s">
+        <v>496</v>
+      </c>
+      <c r="G45" t="s">
+        <v>32</v>
+      </c>
+      <c r="H45" t="s">
+        <v>33</v>
+      </c>
+      <c r="I45" t="s">
+        <v>34</v>
+      </c>
+      <c r="J45" t="s">
+        <v>33</v>
+      </c>
+      <c r="K45" t="s">
+        <v>35</v>
+      </c>
+      <c r="L45" t="s">
+        <v>32</v>
+      </c>
+      <c r="M45" t="s">
+        <v>32</v>
+      </c>
+      <c r="N45" t="s">
+        <v>32</v>
+      </c>
+      <c r="O45" t="s">
+        <v>32</v>
+      </c>
+      <c r="P45" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>497</v>
+      </c>
+      <c r="R45" t="s">
+        <v>111</v>
+      </c>
+      <c r="S45" t="s">
+        <v>498</v>
+      </c>
+      <c r="T45" t="s">
+        <v>499</v>
+      </c>
+      <c r="U45" t="s">
+        <v>500</v>
+      </c>
+      <c r="V45" t="s">
+        <v>501</v>
+      </c>
+      <c r="W45" t="s">
+        <v>502</v>
+      </c>
+      <c r="X45" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>503</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>78</v>
+      </c>
+      <c r="AS45" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT45" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:47" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>504</v>
+      </c>
+      <c r="B46" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" t="s">
+        <v>29</v>
+      </c>
+      <c r="E46" t="s">
+        <v>505</v>
+      </c>
+      <c r="F46" t="s">
+        <v>506</v>
+      </c>
+      <c r="G46" t="s">
+        <v>32</v>
+      </c>
+      <c r="H46" t="s">
+        <v>33</v>
+      </c>
+      <c r="I46" t="s">
+        <v>34</v>
+      </c>
+      <c r="J46" t="s">
+        <v>33</v>
+      </c>
+      <c r="K46" t="s">
+        <v>35</v>
+      </c>
+      <c r="L46" t="s">
+        <v>32</v>
+      </c>
+      <c r="M46" t="s">
+        <v>32</v>
+      </c>
+      <c r="N46" t="s">
+        <v>32</v>
+      </c>
+      <c r="O46" t="s">
+        <v>32</v>
+      </c>
+      <c r="P46" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>507</v>
+      </c>
+      <c r="R46" t="s">
+        <v>50</v>
+      </c>
+      <c r="S46" t="s">
+        <v>508</v>
+      </c>
+      <c r="T46" t="s">
+        <v>509</v>
+      </c>
+      <c r="U46" t="s">
+        <v>75</v>
+      </c>
+      <c r="V46" t="s">
+        <v>510</v>
+      </c>
+      <c r="W46" t="s">
+        <v>511</v>
+      </c>
+      <c r="X46" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>512</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>78</v>
+      </c>
+      <c r="AS46" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT46" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU46" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>